<commit_message>
Add funzionalita non è possibile sforare  crediti
</commit_message>
<xml_diff>
--- a/RecapAsta.xlsx
+++ b/RecapAsta.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabella Squadre" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tabella Squadre" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>a</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>bbb</t>
+          <t>v</t>
         </is>
       </c>
     </row>
@@ -448,36 +448,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RAVAGLIA 1 Sampdoria</t>
+          <t>SILVESTRI 1 Verona</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SZCZESNY 1 Juventus</t>
+          <t>RADU I. 1 Inter</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KRAPIKAS 1 Spezia</t>
+          <t>SKORUPSKI 1 Bologna</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CONTINI 1 Napoli</t>
+          <t>PANDUR 1 Verona</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PROVEDEL 1 Spezia</t>
+          <t>MONTIPO' 1 Benevento</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FESTA 1 Crotone</t>
+          <t>OSPINA 1 Napoli</t>
         </is>
       </c>
     </row>
@@ -496,96 +496,96 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ROMAGNA 1 Sassuolo</t>
+          <t>BIRASCHI 1 Genoa</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZAPPA 1 Cagliari</t>
+          <t>DIMARCO 1 Verona</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IBANEZ 1 Roma</t>
+          <t>FRABOTTA 1 Juventus</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PEZZELLA GIU. 1 Parma</t>
+          <t>RUGANI 1 Cagliari</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MALCUIT 1 Fiorentina</t>
+          <t>FOULON 1 Benevento</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ZAPATA C. 1 Genoa</t>
+          <t>GHISLANDI 1 Atalanta</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RUEGG 1 Verona</t>
+          <t>DARMIAN 1 Inter</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DE LIGT 1 Juventus</t>
+          <t>SINGO 1 Torino</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KUMBULLA 1 Roma</t>
+          <t>DEPAOLI 1 Benevento</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BARBA 1 Benevento</t>
+          <t>PELUSO 1 Sassuolo</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CAPRADOSSI 1 Spezia</t>
+          <t>DIERCKX 1 Parma</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OSORIO 1 Parma</t>
+          <t>ARMINI 1 Lazio</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BASTONI S. 1 Spezia</t>
+          <t>GHOULAM 1 Napoli</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>STRYGER LARSEN 1 Udinese</t>
+          <t>CRISCITO 1 Genoa</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RISPOLI 1 Crotone</t>
+          <t>RODRIGO BECAO 1 Udinese</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SOUMAORO 1 Bologna</t>
+          <t>ROMAGNOLI 1 Milan</t>
         </is>
       </c>
     </row>
@@ -604,96 +604,96 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RAMIREZ 1 Sampdoria</t>
+          <t>LAZOVIC 1 Verona</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MCKENNIE 1 Juventus</t>
+          <t>PASTORE 1 Roma</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SVANBERG 1 Bologna</t>
+          <t>LUCAS LEIVA 1 Lazio</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SCHIATTARELLA 1 Benevento</t>
+          <t>SAPONARA 1 Spezia</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>RUIZ 1 Napoli</t>
+          <t>JANKTO 1 Sampdoria</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SAELEMAEKERS 1 Milan</t>
+          <t>SVANBERG 1 Bologna</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>POLI 1 Bologna</t>
+          <t>BARAK 1 Verona</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>GRASSI 1 Parma</t>
+          <t>LOBOTKA 1 Napoli</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ROVELLA 1 Genoa</t>
+          <t>KULUSEVSKI 1 Juventus</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CALHANOGLU 1 Milan</t>
+          <t>MANDRAGORA 1 Torino</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ZACCAGNI 1 Verona</t>
+          <t>NANDEZ 1 Cagliari</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>PETRICCIONE 1 Crotone</t>
+          <t>KURTIC 1 Parma</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PASALIC 1 Atalanta</t>
+          <t>KUCKA 1 Parma</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PULGAR 1 Fiorentina</t>
+          <t>POLI 1 Bologna</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SCHOUTEN 1 Bologna</t>
+          <t>JAJALO 1 Udinese</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SOTTIL 1 Cagliari</t>
+          <t>ARSLAN 1 Udinese</t>
         </is>
       </c>
     </row>
@@ -712,72 +712,72 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MESSIAS 1 Crotone</t>
+          <t>BRAAF 1 Udinese</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RONALDO 1 Juventus</t>
+          <t>CAPUTO 1 Sassuolo</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>KOUAME' 1 Fiorentina</t>
+          <t>SANCHEZ 1 Inter</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SHOMURODOV 1 Genoa</t>
+          <t>HAUGE 1 Milan</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>ODDEI 1 Sassuolo</t>
+          <t>MONCINI 1 Benevento</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MIHAILA 1 Parma</t>
+          <t>JUWARA 1 Bologna</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SANCHEZ 1 Inter</t>
+          <t>MESSIAS 1 Crotone</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MAYORAL 1 Roma</t>
+          <t>DRAGUS 1 Crotone</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PELLE' 1 Parma</t>
+          <t>INGLESE 1 Parma</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RIBERY 1 Fiorentina</t>
+          <t>LA GUMINA 1 Sampdoria</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NZOLA 1 Spezia</t>
+          <t>ILICIC 1 Atalanta</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BRAAF 1 Udinese</t>
+          <t>DEULOFEU 1 Udinese</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Mod  stile creaExcel e Readme
</commit_message>
<xml_diff>
--- a/RecapAsta.xlsx
+++ b/RecapAsta.xlsx
@@ -17,13 +17,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFF6600"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF0000FF"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF008000"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FFFF0000"/>
+      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +70,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,26 +449,30 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>v</t>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Salernitana</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Napoli</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Portieri</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Portieri</t>
         </is>
@@ -448,46 +481,46 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SILVESTRI 1 Verona</t>
+          <t>PADELLI  --  1  --  Inter</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RADU I. 1 Inter</t>
+          <t>RINALDI  --  1  --  Parma</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SKORUPSKI 1 Bologna</t>
+          <t>RADUNOVIC  --  1  --  Atalanta</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PANDUR 1 Verona</t>
+          <t>SZCZESNY  --  1  --  Juventus</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MONTIPO' 1 Benevento</t>
+          <t>HANDANOVIC  --  1  --  Inter</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OSPINA 1 Napoli</t>
+          <t>SPORTIELLO  --  1  --  Atalanta</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Difensori</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Difensori</t>
         </is>
@@ -496,106 +529,106 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BIRASCHI 1 Genoa</t>
+          <t>MARRONE  --  1  --  Crotone</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DIMARCO 1 Verona</t>
+          <t>KUMBULLA  --  1  --  Roma</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FRABOTTA 1 Juventus</t>
+          <t>GOLDANIGA  --  1  --  Genoa</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RUGANI 1 Cagliari</t>
+          <t>IACOPONI  --  1  --  Parma</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FOULON 1 Benevento</t>
+          <t>RAMOS  --  1  --  Spezia</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>GHISLANDI 1 Atalanta</t>
+          <t>TOMORI  --  1  --  Milan</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DARMIAN 1 Inter</t>
+          <t>TRIPALDELLI  --  1  --  Cagliari</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SINGO 1 Torino</t>
+          <t>CUADRADO  --  1  --  Juventus</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DEPAOLI 1 Benevento</t>
+          <t>PEZZELLA GER.  --  1  --  Fiorentina</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PELUSO 1 Sassuolo</t>
+          <t>YOUNG  --  1  --  Inter</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DIERCKX 1 Parma</t>
+          <t>SMALLING  --  1  --  Roma</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ARMINI 1 Lazio</t>
+          <t>MBAYE  --  1  --  Bologna</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GHOULAM 1 Napoli</t>
+          <t>MURRU  --  1  --  Torino</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CRISCITO 1 Genoa</t>
+          <t>BASTONI  --  1  --  Inter</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RODRIGO BECAO 1 Udinese</t>
+          <t>HATEBOER  --  1  --  Atalanta</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ROMAGNOLI 1 Milan</t>
+          <t>RANOCCHIA  --  1  --  Inter</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="4" t="inlineStr">
         <is>
           <t>Centrocampisti</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="4" t="inlineStr">
         <is>
           <t>Centrocampisti</t>
         </is>
@@ -604,106 +637,106 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LAZOVIC 1 Verona</t>
+          <t>ANDERSON D.  --  1  --  Lazio</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PASTORE 1 Roma</t>
+          <t>ERIKSEN  --  1  --  Inter</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LUCAS LEIVA 1 Lazio</t>
+          <t>BASELLI  --  1  --  Torino</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SAPONARA 1 Spezia</t>
+          <t>LOCATELLI  --  1  --  Sassuolo</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>JANKTO 1 Sampdoria</t>
+          <t>SVANBERG  --  1  --  Bologna</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SVANBERG 1 Bologna</t>
+          <t>ROJAS  --  1  --  Crotone</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BARAK 1 Verona</t>
+          <t>BARELLA  --  1  --  Inter</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LOBOTKA 1 Napoli</t>
+          <t>PEREIRO  --  1  --  Cagliari</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>KULUSEVSKI 1 Juventus</t>
+          <t>GRASSI  --  1  --  Parma</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MANDRAGORA 1 Torino</t>
+          <t>KOVALENKO  --  1  --  Atalanta</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NANDEZ 1 Cagliari</t>
+          <t>KULUSEVSKI  --  1  --  Juventus</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KURTIC 1 Parma</t>
+          <t>MELEGONI  --  1  --  Genoa</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>KUCKA 1 Parma</t>
+          <t>CYPRIEN  --  1  --  Parma</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>POLI 1 Bologna</t>
+          <t>DOMINGUEZ  --  1  --  Bologna</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>JAJALO 1 Udinese</t>
+          <t>AGUDELO  --  1  --  Spezia</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ARSLAN 1 Udinese</t>
+          <t>MIRANCHUK  --  1  --  Atalanta</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="5" t="inlineStr">
         <is>
           <t>Attaccanti</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="5" t="inlineStr">
         <is>
           <t>Attaccanti</t>
         </is>
@@ -712,72 +745,72 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BRAAF 1 Udinese</t>
+          <t>FARIAS  --  1  --  Spezia</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CAPUTO 1 Sassuolo</t>
+          <t>IMMOBILE  --  1  --  Lazio</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SANCHEZ 1 Inter</t>
+          <t>SIMEONE  --  1  --  Cagliari</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>HAUGE 1 Milan</t>
+          <t>KOUAME'  --  1  --  Fiorentina</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MONCINI 1 Benevento</t>
+          <t>RIVIERE  --  1  --  Crotone</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>JUWARA 1 Bologna</t>
+          <t>SAU  --  1  --  Benevento</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MESSIAS 1 Crotone</t>
+          <t>BRAAF  --  1  --  Udinese</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DRAGUS 1 Crotone</t>
+          <t>ZAZA  --  1  --  Torino</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>INGLESE 1 Parma</t>
+          <t>NESTOROVSKI  --  1  --  Udinese</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>LA GUMINA 1 Sampdoria</t>
+          <t>TORREGROSSA  --  1  --  Sampdoria</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ILICIC 1 Atalanta</t>
+          <t>OKAKA  --  1  --  Udinese</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DEULOFEU 1 Udinese</t>
+          <t>PANDEV  --  1  --  Genoa</t>
         </is>
       </c>
     </row>

</xml_diff>